<commit_message>
button colors has been slightly changed. add timeout 3 seconds in axios. leave module has been updated     -> more security added.     -> trim reason has been added.     -> sunday could not be selected as a leave date.     -> loading screens added.     -> new success messages. Employee Profile     -> add status [short leave] in attendance. Attendance Correction     -> UI Updates     -> Validations added.     -> Loading Screens has been added.
</commit_message>
<xml_diff>
--- a/assets/portal/assets/excel/attendance/5000_attendance.xlsx
+++ b/assets/portal/assets/excel/attendance/5000_attendance.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
   <si>
     <t>Sr.No</t>
   </si>
@@ -49,47 +49,41 @@
     <t>Log(s)</t>
   </si>
   <si>
-    <t>Temporary</t>
-  </si>
-  <si>
-    <t>Tue Aug 22 2023</t>
-  </si>
-  <si>
-    <t>11:22:20</t>
-  </si>
-  <si>
-    <t>11:31:51</t>
-  </si>
-  <si>
-    <t>0:9</t>
-  </si>
-  <si>
-    <t>Paid</t>
+    <t>Muhammad Usman</t>
+  </si>
+  <si>
+    <t>Sat Oct 07 2023</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Applied For Leave</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Mon Aug 21 2023</t>
-  </si>
-  <si>
-    <t>14:04:46</t>
-  </si>
-  <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t>Thu Aug 17 2023</t>
-  </si>
-  <si>
-    <t>16:35:00</t>
+    <t>Fri Oct 06 2023</t>
+  </si>
+  <si>
+    <t>Thu Oct 05 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 03 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -102,11 +96,8 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <color rgb="000000"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,11 +112,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="82ca9d"/>
       </patternFill>
     </fill>
   </fills>
@@ -155,15 +141,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -508,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -518,14 +501,15 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" outlineLevel="1" collapsed="1" customWidth="1"/>
-    <col min="2" max="3" width="18" outlineLevel="1" collapsed="1" customWidth="1"/>
+    <col min="2" max="2" width="18" outlineLevel="1" collapsed="1" customWidth="1"/>
+    <col min="3" max="3" width="19" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="4" max="4" width="20" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="5" max="5" width="15" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="6" max="6" width="13" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="7" max="7" width="16" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="8" max="8" width="14" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="9" max="9" width="12" outlineLevel="1" collapsed="1" customWidth="1"/>
-    <col min="10" max="10" width="11" outlineLevel="1" collapsed="1" customWidth="1"/>
+    <col min="10" max="10" width="22" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="11" max="12" width="10" outlineLevel="1" collapsed="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -572,7 +556,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>70001004</v>
+        <v>5000</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -580,23 +564,17 @@
       <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>18</v>
+      <c r="K2" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -604,28 +582,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>70001004</v>
+        <v>5000</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -633,28 +608,103 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>70001004</v>
+        <v>5000</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5000</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5000</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>5000</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>18</v>
+      <c r="I7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Locations Dropdown in Monthly Attendance
</commit_message>
<xml_diff>
--- a/assets/portal/assets/excel/attendance/5000_attendance.xlsx
+++ b/assets/portal/assets/excel/attendance/5000_attendance.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="88">
   <si>
     <t>Sr.No</t>
   </si>
@@ -49,40 +49,232 @@
     <t>Log(s)</t>
   </si>
   <si>
-    <t>Temporary</t>
-  </si>
-  <si>
-    <t>Tue Aug 22 2023</t>
-  </si>
-  <si>
-    <t>11:22:20</t>
-  </si>
-  <si>
-    <t>11:31:51</t>
-  </si>
-  <si>
-    <t>0:9</t>
-  </si>
-  <si>
-    <t>Paid</t>
+    <t>Ahmed Nadeem</t>
+  </si>
+  <si>
+    <t>Wed Nov 16 2022</t>
+  </si>
+  <si>
+    <t>09:12:21</t>
+  </si>
+  <si>
+    <t>17:00:30</t>
+  </si>
+  <si>
+    <t>13:05:25</t>
+  </si>
+  <si>
+    <t>13:22:00</t>
+  </si>
+  <si>
+    <t>7:48</t>
+  </si>
+  <si>
+    <t>Present</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Mon Aug 21 2023</t>
-  </si>
-  <si>
-    <t>14:04:46</t>
+    <t>Antash Javaid</t>
+  </si>
+  <si>
+    <t>10:29:40</t>
+  </si>
+  <si>
+    <t>18:57:23</t>
+  </si>
+  <si>
+    <t>8:27</t>
+  </si>
+  <si>
+    <t>Anus</t>
+  </si>
+  <si>
+    <t>09:28:31</t>
+  </si>
+  <si>
+    <t>18:49:57</t>
+  </si>
+  <si>
+    <t>13:29:53</t>
+  </si>
+  <si>
+    <t>13:56:28</t>
+  </si>
+  <si>
+    <t>9:21</t>
+  </si>
+  <si>
+    <t>Late</t>
+  </si>
+  <si>
+    <t>Fahim</t>
   </si>
   <si>
     <t>---</t>
   </si>
   <si>
-    <t>Thu Aug 17 2023</t>
-  </si>
-  <si>
-    <t>16:35:00</t>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Mahmood ul Hassan</t>
+  </si>
+  <si>
+    <t>Muhammad Ammar Siddiqui</t>
+  </si>
+  <si>
+    <t>09:19:05</t>
+  </si>
+  <si>
+    <t>17:36:44</t>
+  </si>
+  <si>
+    <t>13:06:38</t>
+  </si>
+  <si>
+    <t>14:13:58</t>
+  </si>
+  <si>
+    <t>8:17</t>
+  </si>
+  <si>
+    <t>Muhammad Arif</t>
+  </si>
+  <si>
+    <t>09:17:43</t>
+  </si>
+  <si>
+    <t>17:21:11</t>
+  </si>
+  <si>
+    <t>13:05:42</t>
+  </si>
+  <si>
+    <t>13:27:48</t>
+  </si>
+  <si>
+    <t>8:3</t>
+  </si>
+  <si>
+    <t>Muhammad Faisal</t>
+  </si>
+  <si>
+    <t>10:19:42</t>
+  </si>
+  <si>
+    <t>17:00:38</t>
+  </si>
+  <si>
+    <t>6:40</t>
+  </si>
+  <si>
+    <t>Muhammad Javaid Lakhani</t>
+  </si>
+  <si>
+    <t>08:33:40</t>
+  </si>
+  <si>
+    <t>17:00:48</t>
+  </si>
+  <si>
+    <t>13:27:00</t>
+  </si>
+  <si>
+    <t>13:53:38</t>
+  </si>
+  <si>
+    <t>Muhammad Sarfaraz</t>
+  </si>
+  <si>
+    <t>Muhammad Shehzad Liaquat</t>
+  </si>
+  <si>
+    <t>09:10:23</t>
+  </si>
+  <si>
+    <t>17:11:14</t>
+  </si>
+  <si>
+    <t>13:53:13</t>
+  </si>
+  <si>
+    <t>13:53:48</t>
+  </si>
+  <si>
+    <t>8:0</t>
+  </si>
+  <si>
+    <t>Muhammad Shoaib</t>
+  </si>
+  <si>
+    <t>11:12:58</t>
+  </si>
+  <si>
+    <t>18:45:33</t>
+  </si>
+  <si>
+    <t>7:32</t>
+  </si>
+  <si>
+    <t>Muhammad Zaid</t>
+  </si>
+  <si>
+    <t>09:14:06</t>
+  </si>
+  <si>
+    <t>15:59:28</t>
+  </si>
+  <si>
+    <t>13:27:08</t>
+  </si>
+  <si>
+    <t>13:43:15</t>
+  </si>
+  <si>
+    <t>6:45</t>
+  </si>
+  <si>
+    <t>Salman Ahmed</t>
+  </si>
+  <si>
+    <t>11:55:54</t>
+  </si>
+  <si>
+    <t>18:52:39</t>
+  </si>
+  <si>
+    <t>13:43:38</t>
+  </si>
+  <si>
+    <t>14:01:20</t>
+  </si>
+  <si>
+    <t>6:56</t>
+  </si>
+  <si>
+    <t>Samiullah Farooq</t>
+  </si>
+  <si>
+    <t>10:52:18</t>
+  </si>
+  <si>
+    <t>11:49:38</t>
+  </si>
+  <si>
+    <t>Syed Muhammad Fawad Kareem</t>
+  </si>
+  <si>
+    <t>09:12:03</t>
+  </si>
+  <si>
+    <t>17:15:47</t>
+  </si>
+  <si>
+    <t>13:25:53</t>
+  </si>
+  <si>
+    <t>13:43:06</t>
   </si>
 </sst>
 </file>
@@ -106,7 +298,7 @@
       <color rgb="000000"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,7 +317,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="82ca9d"/>
+        <fgColor rgb="cac7c4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ebcccf"/>
       </patternFill>
     </fill>
   </fills>
@@ -155,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -163,10 +360,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -508,7 +708,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -518,14 +718,14 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" outlineLevel="1" collapsed="1" customWidth="1"/>
-    <col min="2" max="3" width="18" outlineLevel="1" collapsed="1" customWidth="1"/>
+    <col min="2" max="2" width="18" outlineLevel="1" collapsed="1" customWidth="1"/>
+    <col min="3" max="3" width="31" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="4" max="4" width="20" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="5" max="5" width="15" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="6" max="6" width="13" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="7" max="7" width="16" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="8" max="8" width="14" outlineLevel="1" collapsed="1" customWidth="1"/>
-    <col min="9" max="9" width="12" outlineLevel="1" collapsed="1" customWidth="1"/>
-    <col min="10" max="10" width="11" outlineLevel="1" collapsed="1" customWidth="1"/>
+    <col min="9" max="10" width="12" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="11" max="12" width="10" outlineLevel="1" collapsed="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -572,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>70001004</v>
+        <v>20017</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -586,17 +786,23 @@
       <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="L2" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -604,28 +810,31 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>70001004</v>
+        <v>20015</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>18</v>
+      <c r="K3" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -633,28 +842,503 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>70001004</v>
+        <v>20019</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>20011</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>20004</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>20007</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>20003</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>20010</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>20009</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>20006</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>20005</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="B13" s="2">
+        <v>20008</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>20016</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>20013</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>20000</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>20000</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>18</v>
+      <c r="B18" s="2">
+        <v>20002</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fuel equipment (trips) db structure change with multiple requests
</commit_message>
<xml_diff>
--- a/assets/portal/assets/excel/attendance/5000_attendance.xlsx
+++ b/assets/portal/assets/excel/attendance/5000_attendance.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
   <si>
     <t>Sr.No</t>
   </si>
@@ -49,232 +49,163 @@
     <t>Log(s)</t>
   </si>
   <si>
-    <t>Ahmed Nadeem</t>
-  </si>
-  <si>
-    <t>Wed Nov 16 2022</t>
-  </si>
-  <si>
-    <t>09:12:21</t>
-  </si>
-  <si>
-    <t>17:00:30</t>
-  </si>
-  <si>
-    <t>13:05:25</t>
-  </si>
-  <si>
-    <t>13:22:00</t>
-  </si>
-  <si>
-    <t>7:48</t>
+    <t>Abdul Rashid Kath</t>
+  </si>
+  <si>
+    <t>Wed Apr 06 2022</t>
+  </si>
+  <si>
+    <t>10:45:22</t>
+  </si>
+  <si>
+    <t>17:19:24</t>
+  </si>
+  <si>
+    <t>6:34</t>
+  </si>
+  <si>
+    <t>Late</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Asad Ali</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Fahad</t>
+  </si>
+  <si>
+    <t>13:27:17</t>
+  </si>
+  <si>
+    <t>Javid</t>
+  </si>
+  <si>
+    <t>09:42:54</t>
+  </si>
+  <si>
+    <t>Kifayat Ullah</t>
+  </si>
+  <si>
+    <t>Mahesh</t>
+  </si>
+  <si>
+    <t>10:22:00</t>
+  </si>
+  <si>
+    <t>15:05:00</t>
+  </si>
+  <si>
+    <t>4:43</t>
+  </si>
+  <si>
+    <t>Manzoor Hussain</t>
+  </si>
+  <si>
+    <t>09:04:28</t>
+  </si>
+  <si>
+    <t>15:26:03</t>
+  </si>
+  <si>
+    <t>6:21</t>
   </si>
   <si>
     <t>Present</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Antash Javaid</t>
-  </si>
-  <si>
-    <t>10:29:40</t>
-  </si>
-  <si>
-    <t>18:57:23</t>
-  </si>
-  <si>
-    <t>8:27</t>
-  </si>
-  <si>
-    <t>Anus</t>
-  </si>
-  <si>
-    <t>09:28:31</t>
-  </si>
-  <si>
-    <t>18:49:57</t>
-  </si>
-  <si>
-    <t>13:29:53</t>
-  </si>
-  <si>
-    <t>13:56:28</t>
-  </si>
-  <si>
-    <t>9:21</t>
-  </si>
-  <si>
-    <t>Late</t>
-  </si>
-  <si>
-    <t>Fahim</t>
-  </si>
-  <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t>Absent</t>
-  </si>
-  <si>
-    <t>Mahmood ul Hassan</t>
-  </si>
-  <si>
-    <t>Muhammad Ammar Siddiqui</t>
-  </si>
-  <si>
-    <t>09:19:05</t>
-  </si>
-  <si>
-    <t>17:36:44</t>
-  </si>
-  <si>
-    <t>13:06:38</t>
-  </si>
-  <si>
-    <t>14:13:58</t>
-  </si>
-  <si>
-    <t>8:17</t>
-  </si>
-  <si>
-    <t>Muhammad Arif</t>
-  </si>
-  <si>
-    <t>09:17:43</t>
-  </si>
-  <si>
-    <t>17:21:11</t>
-  </si>
-  <si>
-    <t>13:05:42</t>
-  </si>
-  <si>
-    <t>13:27:48</t>
-  </si>
-  <si>
-    <t>8:3</t>
-  </si>
-  <si>
-    <t>Muhammad Faisal</t>
-  </si>
-  <si>
-    <t>10:19:42</t>
-  </si>
-  <si>
-    <t>17:00:38</t>
-  </si>
-  <si>
-    <t>6:40</t>
-  </si>
-  <si>
-    <t>Muhammad Javaid Lakhani</t>
-  </si>
-  <si>
-    <t>08:33:40</t>
-  </si>
-  <si>
-    <t>17:00:48</t>
-  </si>
-  <si>
-    <t>13:27:00</t>
-  </si>
-  <si>
-    <t>13:53:38</t>
-  </si>
-  <si>
-    <t>Muhammad Sarfaraz</t>
-  </si>
-  <si>
-    <t>Muhammad Shehzad Liaquat</t>
-  </si>
-  <si>
-    <t>09:10:23</t>
-  </si>
-  <si>
-    <t>17:11:14</t>
-  </si>
-  <si>
-    <t>13:53:13</t>
-  </si>
-  <si>
-    <t>13:53:48</t>
-  </si>
-  <si>
-    <t>8:0</t>
-  </si>
-  <si>
-    <t>Muhammad Shoaib</t>
-  </si>
-  <si>
-    <t>11:12:58</t>
-  </si>
-  <si>
-    <t>18:45:33</t>
-  </si>
-  <si>
-    <t>7:32</t>
-  </si>
-  <si>
-    <t>Muhammad Zaid</t>
-  </si>
-  <si>
-    <t>09:14:06</t>
-  </si>
-  <si>
-    <t>15:59:28</t>
-  </si>
-  <si>
-    <t>13:27:08</t>
-  </si>
-  <si>
-    <t>13:43:15</t>
-  </si>
-  <si>
-    <t>6:45</t>
-  </si>
-  <si>
-    <t>Salman Ahmed</t>
-  </si>
-  <si>
-    <t>11:55:54</t>
-  </si>
-  <si>
-    <t>18:52:39</t>
-  </si>
-  <si>
-    <t>13:43:38</t>
-  </si>
-  <si>
-    <t>14:01:20</t>
-  </si>
-  <si>
-    <t>6:56</t>
-  </si>
-  <si>
-    <t>Samiullah Farooq</t>
-  </si>
-  <si>
-    <t>10:52:18</t>
-  </si>
-  <si>
-    <t>11:49:38</t>
-  </si>
-  <si>
-    <t>Syed Muhammad Fawad Kareem</t>
-  </si>
-  <si>
-    <t>09:12:03</t>
-  </si>
-  <si>
-    <t>17:15:47</t>
-  </si>
-  <si>
-    <t>13:25:53</t>
-  </si>
-  <si>
-    <t>13:43:06</t>
+    <t>Muhammad Asif Anwar</t>
+  </si>
+  <si>
+    <t>Muhammad Iqbal</t>
+  </si>
+  <si>
+    <t>09:11:50</t>
+  </si>
+  <si>
+    <t>15:02:49</t>
+  </si>
+  <si>
+    <t>5:50</t>
+  </si>
+  <si>
+    <t>Muhammad Kashif Naseer</t>
+  </si>
+  <si>
+    <t>08:51:50</t>
+  </si>
+  <si>
+    <t>15:22:45</t>
+  </si>
+  <si>
+    <t>6:30</t>
+  </si>
+  <si>
+    <t>Raju</t>
+  </si>
+  <si>
+    <t>10:42:26</t>
+  </si>
+  <si>
+    <t>15:05:45</t>
+  </si>
+  <si>
+    <t>4:23</t>
+  </si>
+  <si>
+    <t>Syed Abid Hussain</t>
+  </si>
+  <si>
+    <t>08:47:44</t>
+  </si>
+  <si>
+    <t>15:06:16</t>
+  </si>
+  <si>
+    <t>6:18</t>
+  </si>
+  <si>
+    <t>Usman Ghani</t>
+  </si>
+  <si>
+    <t>08:48:46</t>
+  </si>
+  <si>
+    <t>15:20:51</t>
+  </si>
+  <si>
+    <t>6:32</t>
+  </si>
+  <si>
+    <t>Yousuf Devid</t>
+  </si>
+  <si>
+    <t>10:47:08</t>
+  </si>
+  <si>
+    <t>15:35:46</t>
+  </si>
+  <si>
+    <t>4:48</t>
+  </si>
+  <si>
+    <t>Zeeshan Ahmed Dawood</t>
+  </si>
+  <si>
+    <t>09:00:31</t>
+  </si>
+  <si>
+    <t>15:27:51</t>
+  </si>
+  <si>
+    <t>6:27</t>
   </si>
 </sst>
 </file>
@@ -360,10 +291,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -708,7 +639,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -719,7 +650,7 @@
   <cols>
     <col min="1" max="1" width="10" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="2" max="2" width="18" outlineLevel="1" collapsed="1" customWidth="1"/>
-    <col min="3" max="3" width="31" outlineLevel="1" collapsed="1" customWidth="1"/>
+    <col min="3" max="3" width="27" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="4" max="4" width="20" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="5" max="5" width="15" outlineLevel="1" collapsed="1" customWidth="1"/>
     <col min="6" max="6" width="13" outlineLevel="1" collapsed="1" customWidth="1"/>
@@ -772,7 +703,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>20017</v>
+        <v>10011</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -786,23 +717,17 @@
       <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>20</v>
+      <c r="K2" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -810,31 +735,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>20015</v>
+        <v>10005</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>20</v>
+      <c r="K3" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -842,37 +761,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>20019</v>
+        <v>10004</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="J4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -880,25 +790,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>20011</v>
+        <v>10014</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="I5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="J5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -906,25 +819,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>20004</v>
+        <v>10012</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -932,37 +845,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>20007</v>
+        <v>10007</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -970,37 +877,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>20003</v>
+        <v>10006</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1008,31 +909,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>20010</v>
+        <v>10009</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="I9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K9" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="J9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1040,37 +935,31 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>20009</v>
+        <v>10001</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1078,25 +967,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>20006</v>
+        <v>10002</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="I11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>20</v>
+        <v>44</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1104,37 +999,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>20005</v>
+        <v>10013</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>20</v>
+        <v>48</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1142,31 +1031,31 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>20008</v>
+        <v>10003</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>20</v>
+        <v>52</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1174,37 +1063,31 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>20016</v>
+        <v>10008</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1212,37 +1095,31 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>20013</v>
+        <v>10010</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>20</v>
+        <v>60</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1250,95 +1127,31 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>81</v>
+        <v>62</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>20</v>
+        <v>64</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2">
-        <v>20000</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2">
-        <v>20002</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>